<commit_message>
bug do moq menor que a quantidade corrigido
</commit_message>
<xml_diff>
--- a/melhores cotacoes.xlsx
+++ b/melhores cotacoes.xlsx
@@ -575,20 +575,20 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Simento</t>
+          <t>Elecronic Direct</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0.096</v>
+        <v>0.05</v>
       </c>
       <c r="G4" t="n">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="H4" t="n">
         <v>4</v>
       </c>
       <c r="I4" t="n">
-        <v>48</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5">
@@ -686,20 +686,20 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Ariat</t>
+          <t>Simento</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>0.72</v>
+        <v>0.18</v>
       </c>
       <c r="G7" t="n">
-        <v>1000</v>
+        <v>450</v>
       </c>
       <c r="H7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I7" t="n">
-        <v>720</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8">
@@ -723,20 +723,20 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Ariat</t>
+          <t>Simento</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>0.24</v>
+        <v>0.12</v>
       </c>
       <c r="G8" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H8" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I8" t="n">
-        <v>240</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9">
@@ -797,20 +797,20 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Elecronic Direct</t>
+          <t>Simento</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>0.035</v>
+        <v>0.0098</v>
       </c>
       <c r="G10" t="n">
-        <v>4000</v>
+        <v>500</v>
       </c>
       <c r="H10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I10" t="n">
-        <v>140</v>
+        <v>39.2</v>
       </c>
     </row>
     <row r="11">

</xml_diff>